<commit_message>
Finishing touches on Data Types Chart
</commit_message>
<xml_diff>
--- a/People/Dan/DataTypes.xlsx
+++ b/People/Dan/DataTypes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\Summer Research\Drasil\People\Dan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD5B04D-4573-4A26-BD23-4252AAAE7414}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F841A34-1ED1-43FC-98C6-52B0B1A09993}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="105">
   <si>
     <t>File Name</t>
   </si>
@@ -331,6 +331,15 @@
   </si>
   <si>
     <t>CodeQuantityDict</t>
+  </si>
+  <si>
+    <t>_ctype :: RawContent</t>
+  </si>
+  <si>
+    <t>Document/Core.hs</t>
+  </si>
+  <si>
+    <t>LabelledContent</t>
   </si>
 </sst>
 </file>
@@ -428,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -445,51 +454,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -820,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK30"/>
+  <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="108" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="108" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -866,32 +850,32 @@
       <c r="A1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="21"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="18"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
@@ -978,16 +962,16 @@
       <c r="AB2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="22" t="s">
+      <c r="AC2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="23"/>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="23"/>
-      <c r="AJ2" s="23"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
       <c r="AK2" s="3"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.45">
@@ -1170,13 +1154,13 @@
       <c r="AB7" s="2"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="21" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -1208,9 +1192,9 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="24"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="6" t="s">
         <v>32</v>
       </c>
@@ -1237,9 +1221,9 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="6" t="s">
         <v>86</v>
       </c>
@@ -1272,13 +1256,13 @@
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="22" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1316,9 +1300,9 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A12" s="15"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="18"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="6" t="s">
         <v>37</v>
       </c>
@@ -1473,76 +1457,56 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>83</v>
+      <c r="B15" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P15" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>16</v>
-      </c>
-      <c r="R15" t="s">
-        <v>16</v>
-      </c>
-      <c r="S15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="V15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="X15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>16</v>
+        <v>103</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="Y15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" t="s">
         <v>16</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -1551,6 +1515,12 @@
       <c r="P16" t="s">
         <v>16</v>
       </c>
+      <c r="Q16" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16" t="s">
+        <v>16</v>
+      </c>
       <c r="S16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1560,7 +1530,10 @@
       <c r="V16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="X16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1572,10 +1545,10 @@
         <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>16</v>
@@ -1590,377 +1563,370 @@
       <c r="M17" t="s">
         <v>16</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="N17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="P17" t="s">
         <v>16</v>
       </c>
-      <c r="Q17" t="s">
-        <v>16</v>
-      </c>
-      <c r="R17" t="s">
-        <v>16</v>
-      </c>
       <c r="S17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U17" t="s">
-        <v>16</v>
-      </c>
-      <c r="V17" t="s">
-        <v>16</v>
-      </c>
-      <c r="X17" t="s">
+      <c r="U17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="Y17" t="s">
         <v>16</v>
       </c>
-      <c r="AC17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A18" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+      <c r="M18" t="s">
+        <v>16</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P18" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>16</v>
+      </c>
+      <c r="R18" t="s">
+        <v>16</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U18" t="s">
+        <v>16</v>
+      </c>
+      <c r="V18" t="s">
+        <v>16</v>
+      </c>
+      <c r="X18" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AD18" t="s">
         <v>47</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AE18" t="s">
         <v>48</v>
       </c>
-      <c r="AF17" s="4" t="s">
+      <c r="AF18" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A18" s="15" t="s">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A19" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B19" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C19" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="N18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U18" t="s">
-        <v>16</v>
-      </c>
-      <c r="V18" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="6" t="s">
+      <c r="N19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="N19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U19" t="s">
-        <v>16</v>
-      </c>
-      <c r="V19" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC19" s="1" t="s">
+      <c r="N20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U20" t="s">
+        <v>16</v>
+      </c>
+      <c r="V20" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC20" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A21" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="N20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>16</v>
-      </c>
-      <c r="R20" t="s">
-        <v>16</v>
-      </c>
-      <c r="S20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U20" t="s">
-        <v>16</v>
-      </c>
-      <c r="V20" t="s">
-        <v>16</v>
-      </c>
-      <c r="X20" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A21" s="12" t="s">
+      <c r="N21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>16</v>
+      </c>
+      <c r="R21" t="s">
+        <v>16</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U21" t="s">
+        <v>16</v>
+      </c>
+      <c r="V21" t="s">
+        <v>16</v>
+      </c>
+      <c r="X21" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B22" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D22" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="N21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC21" s="1" t="s">
+      <c r="N22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AD22" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A22" s="10" t="s">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A23" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22" t="s">
-        <v>16</v>
-      </c>
-      <c r="M22" t="s">
-        <v>16</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U22" t="s">
-        <v>16</v>
-      </c>
-      <c r="V22" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A23" s="15" t="s">
+      <c r="H23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" t="s">
+        <v>16</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U23" t="s">
+        <v>16</v>
+      </c>
+      <c r="V23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A24" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B24" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C24" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="N23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P23" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A24" s="15"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="6" t="s">
+      <c r="N24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P24" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G24" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" t="s">
-        <v>16</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P24" t="s">
-        <v>16</v>
-      </c>
-      <c r="U24" t="s">
-        <v>16</v>
-      </c>
-      <c r="V24" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A25" s="15" t="s">
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P25" t="s">
+        <v>16</v>
+      </c>
+      <c r="U25" t="s">
+        <v>16</v>
+      </c>
+      <c r="V25" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A26" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B26" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C26" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" t="s">
-        <v>16</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O25" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>16</v>
-      </c>
-      <c r="R25" t="s">
-        <v>16</v>
-      </c>
-      <c r="S25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="T25" t="s">
-        <v>16</v>
-      </c>
-      <c r="U25" t="s">
-        <v>16</v>
-      </c>
-      <c r="V25" t="s">
-        <v>16</v>
-      </c>
-      <c r="X25" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A26" s="15"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="6" t="s">
+      <c r="H26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" t="s">
+        <v>16</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>16</v>
+      </c>
+      <c r="R26" t="s">
+        <v>16</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T26" t="s">
+        <v>16</v>
+      </c>
+      <c r="U26" t="s">
+        <v>16</v>
+      </c>
+      <c r="V26" t="s">
+        <v>16</v>
+      </c>
+      <c r="X26" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>16</v>
-      </c>
-      <c r="R26" t="s">
-        <v>16</v>
-      </c>
-      <c r="S26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="T26" t="s">
-        <v>16</v>
-      </c>
-      <c r="U26" t="s">
-        <v>16</v>
-      </c>
-      <c r="V26" t="s">
-        <v>16</v>
-      </c>
-      <c r="X26" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A27" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="J27" t="s">
         <v>16</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="O27" t="s">
+        <v>16</v>
+      </c>
       <c r="Q27" t="s">
         <v>16</v>
       </c>
@@ -1970,6 +1936,9 @@
       <c r="S27" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="T27" t="s">
+        <v>16</v>
+      </c>
       <c r="U27" t="s">
         <v>16</v>
       </c>
@@ -1979,7 +1948,7 @@
       <c r="X27" t="s">
         <v>16</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AB27" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1991,10 +1960,19 @@
         <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" t="s">
+        <v>16</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>16</v>
@@ -2029,19 +2007,10 @@
         <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K29" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>16</v>
@@ -2065,9 +2034,6 @@
         <v>16</v>
       </c>
       <c r="AA29" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB29" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2079,35 +2045,94 @@
         <v>83</v>
       </c>
       <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>16</v>
+      </c>
+      <c r="R30" t="s">
+        <v>16</v>
+      </c>
+      <c r="S30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U30" t="s">
+        <v>16</v>
+      </c>
+      <c r="V30" t="s">
+        <v>16</v>
+      </c>
+      <c r="X30" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A31" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="H30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K30" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U30" t="s">
-        <v>16</v>
-      </c>
-      <c r="V30" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB30" t="s">
+      <c r="H31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" t="s">
+        <v>16</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U31" t="s">
+        <v>16</v>
+      </c>
+      <c r="V31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB31" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
     <mergeCell ref="E1:AB1"/>
     <mergeCell ref="AC2:AJ2"/>
     <mergeCell ref="C8:C10"/>
@@ -2116,17 +2141,8 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
   </mergeCells>
-  <conditionalFormatting sqref="AF3:AH3 O3:AD3 E3:N9 O4:AH9 E10:AH53">
+  <conditionalFormatting sqref="AF3:AH3 O3:AD3 E3:N9 O4:AH9 E10:AH54">
     <cfRule type="cellIs" dxfId="5" priority="46" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2134,7 +2150,7 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2 O2:AB2 O3:AD3 D2:N9 O4:AE9 D10:AE103">
+  <conditionalFormatting sqref="A2 O2:AB2 O3:AD3 D2:N9 O4:AE9 D10:AE104">
     <cfRule type="expression" dxfId="3" priority="49">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>